<commit_message>
Add Inner and Outer Wall Curves
</commit_message>
<xml_diff>
--- a/RegenSolver/enginefiles/engineparameters.xlsx
+++ b/RegenSolver/enginefiles/engineparameters.xlsx
@@ -495,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.127</v>
+        <v>0.08889999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.2347046349630462</v>
+        <v>0.2347036970157674</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -527,7 +527,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.01266768697743744</v>
+        <v>0.006207166618944346</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -535,7 +535,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.157375484050397</v>
+        <v>0.1903706805793461</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -551,7 +551,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.07732858432060842</v>
+        <v>0.0443330164364213</v>
       </c>
     </row>
     <row r="16" spans="1:2">

</xml_diff>